<commit_message>
latest version with working APIs and hardcoded front end
</commit_message>
<xml_diff>
--- a/DataModel.xlsx
+++ b/DataModel.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27815"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="62">
   <si>
     <t>Bowler</t>
   </si>
@@ -66,12 +66,6 @@
     <t>size, name, version</t>
   </si>
   <si>
-    <t>mlb_bo_firstname</t>
-  </si>
-  <si>
-    <t>mlb_bo_lastname</t>
-  </si>
-  <si>
     <t>mlb_bo_address</t>
   </si>
   <si>
@@ -102,27 +96,12 @@
     <t>mlb_ga_number</t>
   </si>
   <si>
-    <t>mlb_ga_eventid</t>
-  </si>
-  <si>
-    <t>Event the game is for</t>
-  </si>
-  <si>
     <t>mlb_ga_bowlerid</t>
   </si>
   <si>
-    <t>mlb_bo_id</t>
-  </si>
-  <si>
     <t>Int</t>
   </si>
   <si>
-    <t>unique id (UUID?)</t>
-  </si>
-  <si>
-    <t>Id of bowler</t>
-  </si>
-  <si>
     <t>mlb_ga_score</t>
   </si>
   <si>
@@ -141,9 +120,6 @@
     <t>mlb_fr_gameid</t>
   </si>
   <si>
-    <t>mlb_ga_id</t>
-  </si>
-  <si>
     <t>int</t>
   </si>
   <si>
@@ -177,9 +153,6 @@
     <t>mlb_sc_id</t>
   </si>
   <si>
-    <t>mlb_sc_day</t>
-  </si>
-  <si>
     <t>mlb_sc_type</t>
   </si>
   <si>
@@ -189,18 +162,9 @@
     <t>mlb_ev_seasonid</t>
   </si>
   <si>
-    <t>mlb_ev_year</t>
-  </si>
-  <si>
-    <t>mlb_ev_month</t>
-  </si>
-  <si>
     <t>mlb_sc_bowlerid</t>
   </si>
   <si>
-    <t>not available, sub, bowling, blank?</t>
-  </si>
-  <si>
     <t>mlb_bo_team</t>
   </si>
   <si>
@@ -214,6 +178,45 @@
   </si>
   <si>
     <t>bowler, scorer, captain, deputy, organizer, treasurer</t>
+  </si>
+  <si>
+    <t>mlb_bo_name</t>
+  </si>
+  <si>
+    <t>first and last name; must be unique for each bowler</t>
+  </si>
+  <si>
+    <t>yyyy-mm-dd</t>
+  </si>
+  <si>
+    <t>make this an optional map in the event object?</t>
+  </si>
+  <si>
+    <t>mlb_ga_ev_id</t>
+  </si>
+  <si>
+    <t>unique = event, and detail is a map in the object?</t>
+  </si>
+  <si>
+    <t>YYyy-mm-dd</t>
+  </si>
+  <si>
+    <t>2016-2017</t>
+  </si>
+  <si>
+    <t>mlb_ev_type</t>
+  </si>
+  <si>
+    <t>event id - yyyy-mm-dd</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>name of bowler</t>
+  </si>
+  <si>
+    <t>n/a, sub, bowling, blank?</t>
   </si>
 </sst>
 </file>
@@ -528,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -541,7 +544,7 @@
     <col min="4" max="4" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -552,46 +555,46 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -602,7 +605,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -613,7 +616,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -624,7 +627,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -635,7 +638,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -646,7 +649,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -657,7 +660,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -668,7 +671,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -679,7 +682,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -687,43 +690,55 @@
         <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
         <v>20</v>
       </c>
-      <c r="C14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15" t="s">
-        <v>21</v>
-      </c>
       <c r="C15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+      <c r="E15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="D16" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -731,10 +746,13 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="D17" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -742,247 +760,184 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D18" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C19" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="B20" t="s">
         <v>30</v>
       </c>
       <c r="C20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" t="s">
         <v>37</v>
-      </c>
-      <c r="D20" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C21" t="s">
-        <v>37</v>
-      </c>
-      <c r="D21" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" t="s">
         <v>34</v>
       </c>
-      <c r="B22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C22" t="s">
-        <v>27</v>
+      <c r="G22" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C23" t="s">
-        <v>27</v>
-      </c>
-      <c r="E23" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C24" t="s">
-        <v>37</v>
+        <v>29</v>
+      </c>
+      <c r="D24" t="s">
+        <v>38</v>
+      </c>
+      <c r="G24" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C25" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D25" t="s">
-        <v>42</v>
-      </c>
-      <c r="G25" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="B26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C26" t="s">
-        <v>37</v>
+        <v>29</v>
+      </c>
+      <c r="D26" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="B27" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="C27" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="D27" t="s">
+        <v>45</v>
+      </c>
+      <c r="G27" t="s">
         <v>46</v>
-      </c>
-      <c r="G27" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B28" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="C28" t="s">
-        <v>37</v>
+        <v>29</v>
+      </c>
+      <c r="D28" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C29" t="s">
-        <v>37</v>
+        <v>29</v>
+      </c>
+      <c r="D29" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="C30" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>4</v>
-      </c>
-      <c r="B31" t="s">
-        <v>53</v>
-      </c>
-      <c r="C31" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>4</v>
-      </c>
-      <c r="B32" t="s">
-        <v>48</v>
-      </c>
-      <c r="C32" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>4</v>
-      </c>
-      <c r="B33" t="s">
-        <v>49</v>
-      </c>
-      <c r="C33" t="s">
-        <v>27</v>
-      </c>
-      <c r="D33" t="s">
-        <v>57</v>
-      </c>
-      <c r="G33" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>3</v>
-      </c>
-      <c r="B34" t="s">
-        <v>47</v>
-      </c>
-      <c r="C34" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>3</v>
-      </c>
-      <c r="B35" t="s">
-        <v>54</v>
-      </c>
-      <c r="C35" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>3</v>
-      </c>
-      <c r="B36" t="s">
-        <v>49</v>
-      </c>
-      <c r="C36" t="s">
-        <v>37</v>
-      </c>
-      <c r="D36" t="s">
-        <v>55</v>
-      </c>
-      <c r="G36" t="s">
-        <v>58</v>
+        <v>29</v>
+      </c>
+      <c r="D30" t="s">
+        <v>61</v>
+      </c>
+      <c r="G30" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1032,7 +987,7 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated data model and added peter's spreadsheet example
</commit_message>
<xml_diff>
--- a/DataModel.xlsx
+++ b/DataModel.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="67">
   <si>
     <t>Bowler</t>
   </si>
@@ -217,6 +217,21 @@
   </si>
   <si>
     <t>n/a, sub, bowling, blank?</t>
+  </si>
+  <si>
+    <t>Series</t>
+  </si>
+  <si>
+    <t>mlb_sr_ev_id</t>
+  </si>
+  <si>
+    <t>mlb_sr_bowlerid</t>
+  </si>
+  <si>
+    <t>mlb_sr_highscratch</t>
+  </si>
+  <si>
+    <t>mlb_sr_highwithhandicap</t>
   </si>
 </sst>
 </file>
@@ -531,15 +546,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="22.83203125" customWidth="1"/>
     <col min="3" max="3" width="21.5" customWidth="1"/>
     <col min="4" max="4" width="17.33203125" customWidth="1"/>
   </cols>
@@ -771,10 +786,10 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="C19" t="s">
         <v>22</v>
@@ -782,24 +797,21 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="C20" t="s">
-        <v>22</v>
-      </c>
-      <c r="E20" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="B21" t="s">
-        <v>31</v>
+        <v>65</v>
       </c>
       <c r="C21" t="s">
         <v>29</v>
@@ -807,19 +819,13 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="B22" t="s">
-        <v>32</v>
+        <v>66</v>
       </c>
       <c r="C22" t="s">
         <v>29</v>
-      </c>
-      <c r="D22" t="s">
-        <v>34</v>
-      </c>
-      <c r="G22" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -827,10 +833,10 @@
         <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C23" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -838,105 +844,158 @@
         <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C24" t="s">
-        <v>29</v>
-      </c>
-      <c r="D24" t="s">
-        <v>38</v>
-      </c>
-      <c r="G24" t="s">
-        <v>46</v>
+        <v>22</v>
+      </c>
+      <c r="E24" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C25" t="s">
         <v>29</v>
-      </c>
-      <c r="D25" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C26" t="s">
         <v>29</v>
       </c>
       <c r="D26" t="s">
-        <v>56</v>
+        <v>34</v>
+      </c>
+      <c r="G26" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="C27" t="s">
-        <v>22</v>
-      </c>
-      <c r="D27" t="s">
-        <v>45</v>
-      </c>
-      <c r="G27" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C28" t="s">
         <v>29</v>
       </c>
       <c r="D28" t="s">
-        <v>58</v>
+        <v>38</v>
+      </c>
+      <c r="G28" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B29" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C29" t="s">
         <v>29</v>
       </c>
       <c r="D29" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" t="s">
+        <v>45</v>
+      </c>
+      <c r="G31" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>3</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B32" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" t="s">
+        <v>29</v>
+      </c>
+      <c r="D32" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" t="s">
+        <v>43</v>
+      </c>
+      <c r="C33" t="s">
+        <v>29</v>
+      </c>
+      <c r="D33" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" t="s">
         <v>40</v>
       </c>
-      <c r="C30" t="s">
-        <v>29</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="C34" t="s">
+        <v>29</v>
+      </c>
+      <c r="D34" t="s">
         <v>61</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G34" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>